<commit_message>
Adjusted the license file to credit Dimiter (inspiration) and Martin (creator)
</commit_message>
<xml_diff>
--- a/Spreadsheets/Randomised Branch Sampling.xlsx
+++ b/Spreadsheets/Randomised Branch Sampling.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Dropbox/Agile/Forecasting/Focused Objective resources/Spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Dropbox\Private\GitHub\FocusedObjective.Resources\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="2760" windowWidth="27860" windowHeight="17540" activeTab="2"/>
+    <workbookView xWindow="4725" yWindow="2760" windowWidth="27855" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -28,20 +28,20 @@
     <definedName name="StorySamples">RBS!$E$60:$E$70</definedName>
     <definedName name="WeeksToForecast">RBS!$G$24</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Version history -</t>
   </si>
@@ -141,14 +141,17 @@
   <si>
     <t>Stories</t>
   </si>
+  <si>
+    <t>Adjusted the license page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -300,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,9 +319,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -331,8 +331,11 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -362,7 +365,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -411,37 +414,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,37 +456,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,11 +502,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2057023760"/>
-        <c:axId val="-2132069392"/>
+        <c:axId val="436419784"/>
+        <c:axId val="436417040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2057023760"/>
+        <c:axId val="436419784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132069392"/>
+        <c:crossAx val="436417040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -554,7 +557,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132069392"/>
+        <c:axId val="436417040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057023760"/>
+        <c:crossAx val="436419784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -657,7 +660,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -706,37 +709,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -748,37 +751,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -794,11 +797,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2141618176"/>
-        <c:axId val="-2028891280"/>
+        <c:axId val="436417432"/>
+        <c:axId val="436408416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141618176"/>
+        <c:axId val="436417432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,7 +844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028891280"/>
+        <c:crossAx val="436408416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -849,7 +852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028891280"/>
+        <c:axId val="436408416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141618176"/>
+        <c:crossAx val="436417432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -952,7 +955,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1001,37 +1004,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,37 +1046,37 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000.0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3000.0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1089,11 +1092,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2141364736"/>
-        <c:axId val="-2056507360"/>
+        <c:axId val="436418216"/>
+        <c:axId val="436409200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141364736"/>
+        <c:axId val="436418216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,7 +1139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056507360"/>
+        <c:crossAx val="436409200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1144,7 +1147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2056507360"/>
+        <c:axId val="436409200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1198,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141364736"/>
+        <c:crossAx val="436418216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1247,7 +1250,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1296,37 +1299,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1338,37 +1341,37 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1000.0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9000.0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12000.0</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25000.0</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20000.0</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24000.0</c:v>
+                  <c:v>24000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16000.0</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13000.0</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26000.0</c:v>
+                  <c:v>26000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24000.0</c:v>
+                  <c:v>24000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1384,11 +1387,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2029373312"/>
-        <c:axId val="-2059197904"/>
+        <c:axId val="210328824"/>
+        <c:axId val="506816880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029373312"/>
+        <c:axId val="210328824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1434,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059197904"/>
+        <c:crossAx val="506816880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1439,7 +1442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2059197904"/>
+        <c:axId val="506816880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1490,7 +1493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2029373312"/>
+        <c:crossAx val="210328824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3939,7 +3942,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6219825" cy="1877052"/>
+    <xdr:ext cx="6219825" cy="1704826"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -3947,8 +3950,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="685800" y="371474"/>
-          <a:ext cx="6219825" cy="1877052"/>
+          <a:off x="666750" y="371474"/>
+          <a:ext cx="6219825" cy="1704826"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4006,7 +4009,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Throughput Forecasting Tool by </a:t>
+            <a:t>Randomised Branch Sampling spreadsheet tool by Martin Aspeli (@optilude) based on work by </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dimitar Bakardzhiev (@dimiterbak) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>is licensed under a </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -4019,31 +4046,6 @@
               <a:cs typeface="+mn-cs"/>
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
             </a:rPr>
-            <a:t>Focused Objective LLC</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> is licensed under a </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
             <a:t>Creative Commons Attribution-NonCommercial-ShareAlike 4.0 International License</a:t>
           </a:r>
           <a:r>
@@ -4058,56 +4060,18 @@
             </a:rPr>
             <a:t>.</a:t>
           </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Based on a work at</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>https://github.com/FocusedObjective/FocusedObjective.Resources</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" i="0">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -7254,25 +7218,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B23:C24"/>
+  <dimension ref="B23:C25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -7289,7 +7261,7 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7300,229 +7272,229 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
-    <row r="3" spans="2:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="R4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>100</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="R5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="R6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>4</v>
+      <c r="C11" s="7">
+        <f t="shared" ref="C11:C21" ca="1" si="0">RANDBETWEEN(1,NumEpics)</f>
+        <v>74</v>
       </c>
       <c r="D11" s="3">
         <v>32</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>10</v>
+      <c r="C12" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
       </c>
       <c r="D12" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>11</v>
+      <c r="C13" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
       </c>
       <c r="D13" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>3</v>
+      <c r="C14" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
       <c r="D14" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>74</v>
+      <c r="C15" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="D15" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>96</v>
+      <c r="C16" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D16" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>7</v>
       </c>
-      <c r="C17" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>34</v>
+      <c r="C17" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="D17" s="3">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>8</v>
       </c>
-      <c r="C18" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>34</v>
+      <c r="C18" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
       </c>
       <c r="D18" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>9</v>
       </c>
-      <c r="C19" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>2</v>
+      <c r="C19" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="D19" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>10</v>
       </c>
-      <c r="C20" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>30</v>
+      <c r="C20" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="D20" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>11</v>
       </c>
-      <c r="C21" s="8">
-        <f ca="1">RANDBETWEEN(1,NumEpics)</f>
-        <v>93</v>
+      <c r="C21" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
       </c>
       <c r="D21" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="24" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -7530,149 +7502,149 @@
       <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="8">
-        <f>INDEX(EpicSamples,B27)</f>
+      <c r="C27" s="7">
+        <f t="shared" ref="C27:C37" si="1">INDEX(EpicSamples,B27)</f>
         <v>32</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" s="8">
-        <f>INDEX(EpicSamples,B28)</f>
+      <c r="C28" s="7">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29" s="8">
-        <f>INDEX(EpicSamples,B29)</f>
+      <c r="C29" s="7">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>4</v>
       </c>
-      <c r="C30" s="8">
-        <f>INDEX(EpicSamples,B30)</f>
+      <c r="C30" s="7">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>5</v>
       </c>
-      <c r="C31" s="8">
-        <f>INDEX(EpicSamples,B31)</f>
+      <c r="C31" s="7">
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>6</v>
       </c>
-      <c r="C32" s="8">
-        <f>INDEX(EpicSamples,B32)</f>
+      <c r="C32" s="7">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>7</v>
       </c>
-      <c r="C33" s="8">
-        <f>INDEX(EpicSamples,B33)</f>
+      <c r="C33" s="7">
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>8</v>
       </c>
-      <c r="C34" s="8">
-        <f>INDEX(EpicSamples,B34)</f>
+      <c r="C34" s="7">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>9</v>
       </c>
-      <c r="C35" s="8">
-        <f>INDEX(EpicSamples,B35)</f>
+      <c r="C35" s="7">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>10</v>
       </c>
-      <c r="C36" s="8">
-        <f>INDEX(EpicSamples,B36)</f>
+      <c r="C36" s="7">
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>11</v>
       </c>
-      <c r="C37" s="8">
-        <f>INDEX(EpicSamples,B37)</f>
+      <c r="C37" s="7">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+    <row r="40" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B40" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="9"/>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="8"/>
       <c r="C42" s="1" t="s">
         <v>6</v>
       </c>
@@ -7685,7 +7657,7 @@
       <c r="G42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I42" s="11">
+      <c r="I42" s="10">
         <f>(1/COUNT(EpicSamples))*SUM(ProjectStoryEstimates)</f>
         <v>2727.2727272727275</v>
       </c>
@@ -7693,201 +7665,201 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>1</v>
       </c>
-      <c r="C43" s="8">
-        <f>INDEX(EpicSamples,B43)</f>
+      <c r="C43" s="7">
+        <f t="shared" ref="C43:C53" si="2">INDEX(EpicSamples,B43)</f>
         <v>32</v>
       </c>
-      <c r="D43" s="8">
-        <f>INDEX(EpicStories,B43)</f>
+      <c r="D43" s="7">
+        <f t="shared" ref="D43:D53" si="3">INDEX(EpicStories,B43)</f>
         <v>10</v>
       </c>
-      <c r="E43" s="11">
-        <f>D43/(1/NumEpics)</f>
+      <c r="E43" s="10">
+        <f t="shared" ref="E43:E53" si="4">D43/(1/NumEpics)</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44" s="8">
-        <f>INDEX(EpicSamples,B44)</f>
+      <c r="C44" s="7">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="D44" s="8">
-        <f>INDEX(EpicStories,B44)</f>
+      <c r="D44" s="7">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E44" s="11">
-        <f>D44/(1/NumEpics)</f>
+      <c r="E44" s="10">
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>3</v>
       </c>
-      <c r="C45" s="8">
-        <f>INDEX(EpicSamples,B45)</f>
+      <c r="C45" s="7">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="D45" s="8">
-        <f>INDEX(EpicStories,B45)</f>
+      <c r="D45" s="7">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="E45" s="11">
-        <f>D45/(1/NumEpics)</f>
+      <c r="E45" s="10">
+        <f t="shared" si="4"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>4</v>
       </c>
-      <c r="C46" s="8">
-        <f>INDEX(EpicSamples,B46)</f>
+      <c r="C46" s="7">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="D46" s="8">
-        <f>INDEX(EpicStories,B46)</f>
+      <c r="D46" s="7">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="E46" s="11">
-        <f>D46/(1/NumEpics)</f>
+      <c r="E46" s="10">
+        <f t="shared" si="4"/>
         <v>4000</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>5</v>
       </c>
-      <c r="C47" s="8">
-        <f>INDEX(EpicSamples,B47)</f>
+      <c r="C47" s="7">
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
-      <c r="D47" s="8">
-        <f>INDEX(EpicStories,B47)</f>
+      <c r="D47" s="7">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="E47" s="11">
-        <f>D47/(1/NumEpics)</f>
+      <c r="E47" s="10">
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>6</v>
       </c>
-      <c r="C48" s="8">
-        <f>INDEX(EpicSamples,B48)</f>
+      <c r="C48" s="7">
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="D48" s="8">
-        <f>INDEX(EpicStories,B48)</f>
+      <c r="D48" s="7">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="E48" s="11">
-        <f>D48/(1/NumEpics)</f>
+      <c r="E48" s="10">
+        <f t="shared" si="4"/>
         <v>4000</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>7</v>
       </c>
-      <c r="C49" s="8">
-        <f>INDEX(EpicSamples,B49)</f>
+      <c r="C49" s="7">
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="D49" s="8">
-        <f>INDEX(EpicStories,B49)</f>
+      <c r="D49" s="7">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="E49" s="11">
-        <f>D49/(1/NumEpics)</f>
+      <c r="E49" s="10">
+        <f t="shared" si="4"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>8</v>
       </c>
-      <c r="C50" s="8">
-        <f>INDEX(EpicSamples,B50)</f>
+      <c r="C50" s="7">
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="D50" s="8">
-        <f>INDEX(EpicStories,B50)</f>
+      <c r="D50" s="7">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E50" s="11">
-        <f>D50/(1/NumEpics)</f>
+      <c r="E50" s="10">
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>9</v>
       </c>
-      <c r="C51" s="8">
-        <f>INDEX(EpicSamples,B51)</f>
+      <c r="C51" s="7">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D51" s="8">
-        <f>INDEX(EpicStories,B51)</f>
+      <c r="D51" s="7">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="E51" s="11">
-        <f>D51/(1/NumEpics)</f>
+      <c r="E51" s="10">
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>10</v>
       </c>
-      <c r="C52" s="8">
-        <f>INDEX(EpicSamples,B52)</f>
+      <c r="C52" s="7">
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="D52" s="8">
-        <f>INDEX(EpicStories,B52)</f>
+      <c r="D52" s="7">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E52" s="11">
-        <f>D52/(1/NumEpics)</f>
+      <c r="E52" s="10">
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>11</v>
       </c>
-      <c r="C53" s="8">
-        <f>INDEX(EpicSamples,B53)</f>
+      <c r="C53" s="7">
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="D53" s="8">
-        <f>INDEX(EpicStories,B53)</f>
+      <c r="D53" s="7">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="E53" s="11">
-        <f>D53/(1/NumEpics)</f>
+      <c r="E53" s="10">
+        <f t="shared" si="4"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="70" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
+    <row r="56" spans="2:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B57" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B59" s="9"/>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
       <c r="C59" s="1" t="s">
         <v>6</v>
       </c>
@@ -7897,197 +7869,197 @@
       <c r="E59" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="G59" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>1</v>
       </c>
-      <c r="C60" s="8">
-        <f>INDEX(EpicSamples,B60)</f>
+      <c r="C60" s="7">
+        <f t="shared" ref="C60:C70" si="5">INDEX(EpicSamples,B60)</f>
         <v>32</v>
       </c>
-      <c r="D60" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B60))</f>
-        <v>7</v>
+      <c r="D60" s="7">
+        <f t="shared" ref="D60:D70" ca="1" si="6">RANDBETWEEN(1,INDEX(EpicStories,B60))</f>
+        <v>2</v>
       </c>
       <c r="E60" s="3">
         <v>9</v>
       </c>
-      <c r="G60" s="7" t="s">
+      <c r="G60" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>2</v>
       </c>
-      <c r="C61" s="8">
-        <f>INDEX(EpicSamples,B61)</f>
+      <c r="C61" s="7">
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="D61" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B61))</f>
-        <v>13</v>
+      <c r="D61" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
       </c>
       <c r="E61" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>3</v>
       </c>
-      <c r="C62" s="8">
-        <f>INDEX(EpicSamples,B62)</f>
+      <c r="C62" s="7">
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="D62" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B62))</f>
-        <v>20</v>
+      <c r="D62" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>19</v>
       </c>
       <c r="E62" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>4</v>
       </c>
-      <c r="C63" s="8">
-        <f>INDEX(EpicSamples,B63)</f>
+      <c r="C63" s="7">
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="D63" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B63))</f>
-        <v>39</v>
+      <c r="D63" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>24</v>
       </c>
       <c r="E63" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>5</v>
       </c>
-      <c r="C64" s="8">
-        <f>INDEX(EpicSamples,B64)</f>
+      <c r="C64" s="7">
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
-      <c r="D64" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B64))</f>
-        <v>6</v>
+      <c r="D64" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>43</v>
       </c>
       <c r="E64" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>6</v>
       </c>
-      <c r="C65" s="8">
-        <f>INDEX(EpicSamples,B65)</f>
+      <c r="C65" s="7">
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="D65" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B65))</f>
-        <v>19</v>
+      <c r="D65" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>9</v>
       </c>
       <c r="E65" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>7</v>
       </c>
-      <c r="C66" s="8">
-        <f>INDEX(EpicSamples,B66)</f>
+      <c r="C66" s="7">
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
-      <c r="D66" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B66))</f>
-        <v>24</v>
+      <c r="D66" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>9</v>
       </c>
       <c r="E66" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>8</v>
       </c>
-      <c r="C67" s="8">
-        <f>INDEX(EpicSamples,B67)</f>
+      <c r="C67" s="7">
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="D67" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B67))</f>
-        <v>9</v>
+      <c r="D67" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>14</v>
       </c>
       <c r="E67" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>9</v>
       </c>
-      <c r="C68" s="8">
-        <f>INDEX(EpicSamples,B68)</f>
+      <c r="C68" s="7">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="D68" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B68))</f>
-        <v>10</v>
+      <c r="D68" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
       </c>
       <c r="E68" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>10</v>
       </c>
-      <c r="C69" s="8">
-        <f>INDEX(EpicSamples,B69)</f>
+      <c r="C69" s="7">
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="D69" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B69))</f>
-        <v>8</v>
+      <c r="D69" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
       </c>
       <c r="E69" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>11</v>
       </c>
-      <c r="C70" s="8">
-        <f>INDEX(EpicSamples,B70)</f>
+      <c r="C70" s="7">
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="D70" s="8">
-        <f ca="1">RANDBETWEEN(1,INDEX(EpicStories,B70))</f>
-        <v>25</v>
+      <c r="D70" s="7">
+        <f t="shared" ca="1" si="6"/>
+        <v>24</v>
       </c>
       <c r="E70" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B73" s="5" t="str">
+    <row r="73" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B73" s="4" t="str">
         <f>CONCATENATE("Step 5: Estimate the size of each of the sampled stories in ", EstimateType)</f>
         <v>Step 5: Estimate the size of each of the sampled stories in Story Points</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B75" s="9"/>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="8"/>
       <c r="C75" s="1" t="s">
         <v>6</v>
       </c>
@@ -8098,194 +8070,194 @@
         <f>EstimateType</f>
         <v>Story Points</v>
       </c>
-      <c r="G75" s="7" t="s">
+      <c r="G75" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>1</v>
       </c>
-      <c r="C76" s="8">
-        <f>INDEX(EpicSamples,B76)</f>
+      <c r="C76" s="7">
+        <f t="shared" ref="C76:C86" si="7">INDEX(EpicSamples,B76)</f>
         <v>32</v>
       </c>
-      <c r="D76" s="8">
-        <f>INDEX(StorySamples,B76)</f>
+      <c r="D76" s="7">
+        <f t="shared" ref="D76:D86" si="8">INDEX(StorySamples,B76)</f>
         <v>9</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>2</v>
       </c>
-      <c r="C77" s="8">
-        <f>INDEX(EpicSamples,B77)</f>
+      <c r="C77" s="7">
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
-      <c r="D77" s="8">
-        <f>INDEX(StorySamples,B77)</f>
+      <c r="D77" s="7">
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>3</v>
       </c>
-      <c r="C78" s="8">
-        <f>INDEX(EpicSamples,B78)</f>
+      <c r="C78" s="7">
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="D78" s="8">
-        <f>INDEX(StorySamples,B78)</f>
+      <c r="D78" s="7">
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>4</v>
       </c>
-      <c r="C79" s="8">
-        <f>INDEX(EpicSamples,B79)</f>
+      <c r="C79" s="7">
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="D79" s="8">
-        <f>INDEX(StorySamples,B79)</f>
+      <c r="D79" s="7">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>5</v>
       </c>
-      <c r="C80" s="8">
-        <f>INDEX(EpicSamples,B80)</f>
+      <c r="C80" s="7">
+        <f t="shared" si="7"/>
         <v>87</v>
       </c>
-      <c r="D80" s="8">
-        <f>INDEX(StorySamples,B80)</f>
+      <c r="D80" s="7">
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>6</v>
       </c>
-      <c r="C81" s="8">
-        <f>INDEX(EpicSamples,B81)</f>
+      <c r="C81" s="7">
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="D81" s="8">
-        <f>INDEX(StorySamples,B81)</f>
+      <c r="D81" s="7">
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>7</v>
       </c>
-      <c r="C82" s="8">
-        <f>INDEX(EpicSamples,B82)</f>
+      <c r="C82" s="7">
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
-      <c r="D82" s="8">
-        <f>INDEX(StorySamples,B82)</f>
+      <c r="D82" s="7">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>8</v>
       </c>
-      <c r="C83" s="8">
-        <f>INDEX(EpicSamples,B83)</f>
+      <c r="C83" s="7">
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
-      <c r="D83" s="8">
-        <f>INDEX(StorySamples,B83)</f>
+      <c r="D83" s="7">
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>9</v>
       </c>
-      <c r="C84" s="8">
-        <f>INDEX(EpicSamples,B84)</f>
+      <c r="C84" s="7">
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="D84" s="8">
-        <f>INDEX(StorySamples,B84)</f>
+      <c r="D84" s="7">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>10</v>
       </c>
-      <c r="C85" s="8">
-        <f>INDEX(EpicSamples,B85)</f>
+      <c r="C85" s="7">
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
-      <c r="D85" s="8">
-        <f>INDEX(StorySamples,B85)</f>
+      <c r="D85" s="7">
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>11</v>
       </c>
-      <c r="C86" s="8">
-        <f>INDEX(EpicSamples,B86)</f>
+      <c r="C86" s="7">
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
-      <c r="D86" s="8">
-        <f>INDEX(StorySamples,B86)</f>
+      <c r="D86" s="7">
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E86" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="B89" s="5" t="str">
+    <row r="89" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B89" s="4" t="str">
         <f>CONCATENATE("OUTPUT: Estimate the total number of ", EstimateType, " in the project")</f>
         <v>OUTPUT: Estimate the total number of Story Points in the project</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B91" s="9"/>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
       <c r="C91" s="1" t="s">
         <v>6</v>
       </c>
@@ -8305,7 +8277,7 @@
       <c r="I91" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K91" s="11">
+      <c r="K91" s="10">
         <f>(1/COUNT(EpicSamples))*SUM(ProjectEstimates)</f>
         <v>15636.363636363636</v>
       </c>
@@ -8314,278 +8286,278 @@
         <v>Story Points</v>
       </c>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>1</v>
       </c>
-      <c r="C92" s="8">
-        <f>INDEX(EpicSamples,B92)</f>
+      <c r="C92" s="7">
+        <f t="shared" ref="C92:C102" si="9">INDEX(EpicSamples,B92)</f>
         <v>32</v>
       </c>
-      <c r="D92" s="8">
-        <f>INDEX(EpicStories,B92)</f>
+      <c r="D92" s="7">
+        <f t="shared" ref="D92:D102" si="10">INDEX(EpicStories,B92)</f>
         <v>10</v>
       </c>
-      <c r="E92" s="8">
-        <f>INDEX(StorySamples,B92)</f>
+      <c r="E92" s="7">
+        <f t="shared" ref="E92:E102" si="11">INDEX(StorySamples,B92)</f>
         <v>9</v>
       </c>
-      <c r="F92" s="10">
-        <f>INDEX(EstimateSamples,B92)</f>
+      <c r="F92" s="9">
+        <f t="shared" ref="F92:F102" si="12">INDEX(EstimateSamples,B92)</f>
         <v>1</v>
       </c>
-      <c r="G92" s="11">
-        <f>F92/((1/NumEpics)*(1/D92))</f>
+      <c r="G92" s="10">
+        <f t="shared" ref="G92:G102" si="13">F92/((1/NumEpics)*(1/D92))</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>2</v>
       </c>
-      <c r="C93" s="8">
-        <f>INDEX(EpicSamples,B93)</f>
+      <c r="C93" s="7">
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="D93" s="8">
-        <f>INDEX(EpicStories,B93)</f>
+      <c r="D93" s="7">
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
-      <c r="E93" s="8">
-        <f>INDEX(StorySamples,B93)</f>
+      <c r="E93" s="7">
+        <f t="shared" si="11"/>
         <v>18</v>
       </c>
-      <c r="F93" s="10">
-        <f>INDEX(EstimateSamples,B93)</f>
+      <c r="F93" s="9">
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="G93" s="11">
-        <f>F93/((1/NumEpics)*(1/D93))</f>
+      <c r="G93" s="10">
+        <f t="shared" si="13"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>3</v>
       </c>
-      <c r="C94" s="8">
-        <f>INDEX(EpicSamples,B94)</f>
+      <c r="C94" s="7">
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="D94" s="8">
-        <f>INDEX(EpicStories,B94)</f>
+      <c r="D94" s="7">
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
-      <c r="E94" s="8">
-        <f>INDEX(StorySamples,B94)</f>
+      <c r="E94" s="7">
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
-      <c r="F94" s="10">
-        <f>INDEX(EstimateSamples,B94)</f>
+      <c r="F94" s="9">
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="G94" s="11">
-        <f>F94/((1/NumEpics)*(1/D94))</f>
+      <c r="G94" s="10">
+        <f t="shared" si="13"/>
         <v>9000</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>4</v>
       </c>
-      <c r="C95" s="8">
-        <f>INDEX(EpicSamples,B95)</f>
+      <c r="C95" s="7">
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
-      <c r="D95" s="8">
-        <f>INDEX(EpicStories,B95)</f>
+      <c r="D95" s="7">
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="E95" s="8">
-        <f>INDEX(StorySamples,B95)</f>
+      <c r="E95" s="7">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="F95" s="10">
-        <f>INDEX(EstimateSamples,B95)</f>
+      <c r="F95" s="9">
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="G95" s="11">
-        <f>F95/((1/NumEpics)*(1/D95))</f>
+      <c r="G95" s="10">
+        <f t="shared" si="13"/>
         <v>12000</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>5</v>
       </c>
-      <c r="C96" s="8">
-        <f>INDEX(EpicSamples,B96)</f>
+      <c r="C96" s="7">
+        <f t="shared" si="9"/>
         <v>87</v>
       </c>
-      <c r="D96" s="8">
-        <f>INDEX(EpicStories,B96)</f>
+      <c r="D96" s="7">
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="E96" s="8">
-        <f>INDEX(StorySamples,B96)</f>
+      <c r="E96" s="7">
+        <f t="shared" si="11"/>
         <v>34</v>
       </c>
-      <c r="F96" s="10">
-        <f>INDEX(EstimateSamples,B96)</f>
+      <c r="F96" s="9">
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G96" s="11">
-        <f>F96/((1/NumEpics)*(1/D96))</f>
+      <c r="G96" s="10">
+        <f t="shared" si="13"/>
         <v>25000</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>6</v>
       </c>
-      <c r="C97" s="8">
-        <f>INDEX(EpicSamples,B97)</f>
+      <c r="C97" s="7">
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="D97" s="8">
-        <f>INDEX(EpicStories,B97)</f>
+      <c r="D97" s="7">
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="E97" s="8">
-        <f>INDEX(StorySamples,B97)</f>
+      <c r="E97" s="7">
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
-      <c r="F97" s="10">
-        <f>INDEX(EstimateSamples,B97)</f>
+      <c r="F97" s="9">
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G97" s="11">
-        <f>F97/((1/NumEpics)*(1/D97))</f>
+      <c r="G97" s="10">
+        <f t="shared" si="13"/>
         <v>20000</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>7</v>
       </c>
-      <c r="C98" s="8">
-        <f>INDEX(EpicSamples,B98)</f>
+      <c r="C98" s="7">
+        <f t="shared" si="9"/>
         <v>79</v>
       </c>
-      <c r="D98" s="8">
-        <f>INDEX(EpicStories,B98)</f>
+      <c r="D98" s="7">
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
-      <c r="E98" s="8">
-        <f>INDEX(StorySamples,B98)</f>
+      <c r="E98" s="7">
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F98" s="10">
-        <f>INDEX(EstimateSamples,B98)</f>
+      <c r="F98" s="9">
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="G98" s="11">
-        <f>F98/((1/NumEpics)*(1/D98))</f>
+      <c r="G98" s="10">
+        <f t="shared" si="13"/>
         <v>24000</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>8</v>
       </c>
-      <c r="C99" s="8">
-        <f>INDEX(EpicSamples,B99)</f>
+      <c r="C99" s="7">
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="D99" s="8">
-        <f>INDEX(EpicStories,B99)</f>
+      <c r="D99" s="7">
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
-      <c r="E99" s="8">
-        <f>INDEX(StorySamples,B99)</f>
+      <c r="E99" s="7">
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="F99" s="10">
-        <f>INDEX(EstimateSamples,B99)</f>
+      <c r="F99" s="9">
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="G99" s="11">
-        <f>F99/((1/NumEpics)*(1/D99))</f>
+      <c r="G99" s="10">
+        <f t="shared" si="13"/>
         <v>16000</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>9</v>
       </c>
-      <c r="C100" s="8">
-        <f>INDEX(EpicSamples,B100)</f>
+      <c r="C100" s="7">
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="D100" s="8">
-        <f>INDEX(EpicStories,B100)</f>
+      <c r="D100" s="7">
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="E100" s="8">
-        <f>INDEX(StorySamples,B100)</f>
+      <c r="E100" s="7">
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="F100" s="10">
-        <f>INDEX(EstimateSamples,B100)</f>
+      <c r="F100" s="9">
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="G100" s="11">
-        <f>F100/((1/NumEpics)*(1/D100))</f>
+      <c r="G100" s="10">
+        <f t="shared" si="13"/>
         <v>13000</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>10</v>
       </c>
-      <c r="C101" s="8">
-        <f>INDEX(EpicSamples,B101)</f>
+      <c r="C101" s="7">
+        <f t="shared" si="9"/>
         <v>53</v>
       </c>
-      <c r="D101" s="8">
-        <f>INDEX(EpicStories,B101)</f>
+      <c r="D101" s="7">
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
-      <c r="E101" s="8">
-        <f>INDEX(StorySamples,B101)</f>
+      <c r="E101" s="7">
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="F101" s="10">
-        <f>INDEX(EstimateSamples,B101)</f>
+      <c r="F101" s="9">
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="G101" s="11">
-        <f>F101/((1/NumEpics)*(1/D101))</f>
+      <c r="G101" s="10">
+        <f t="shared" si="13"/>
         <v>26000</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>11</v>
       </c>
-      <c r="C102" s="8">
-        <f>INDEX(EpicSamples,B102)</f>
+      <c r="C102" s="7">
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
-      <c r="D102" s="8">
-        <f>INDEX(EpicStories,B102)</f>
+      <c r="D102" s="7">
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
-      <c r="E102" s="8">
-        <f>INDEX(StorySamples,B102)</f>
+      <c r="E102" s="7">
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
-      <c r="F102" s="10">
-        <f>INDEX(EstimateSamples,B102)</f>
+      <c r="F102" s="9">
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="G102" s="11">
-        <f>F102/((1/NumEpics)*(1/D102))</f>
+      <c r="G102" s="10">
+        <f t="shared" si="13"/>
         <v>24000</v>
       </c>
     </row>

</xml_diff>